<commit_message>
update asplos raw data excel
</commit_message>
<xml_diff>
--- a/npb/data/asplos-unicifo.xlsx
+++ b/npb/data/asplos-unicifo.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26404"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26405"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D215342-1E51-4593-A4CC-3614086FC229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{03F0B80D-4DED-4F40-9CCE-238B6794948B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="x86" sheetId="1" r:id="rId1"/>
+    <sheet name="arm" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>class</t>
   </si>
@@ -123,9 +124,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,8 +442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -488,19 +488,18 @@
       <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <f>F2/G2</f>
         <v>0.97049998799836901</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <f>H2/I2</f>
         <v>0.98164565293286099</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <f>J2/K2</f>
         <v>0.95994979157042448</v>
       </c>
-      <c r="E2" s="1"/>
       <c r="F2">
         <v>80.864000000000004</v>
       </c>
@@ -524,19 +523,18 @@
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
         <f>F3/G3</f>
         <v>0.9813567476545586</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <f>H3/I3</f>
         <v>0.98266714833153046</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <f>J3/K3</f>
         <v>0.97773455296785761</v>
       </c>
-      <c r="E3" s="1"/>
       <c r="F3">
         <v>65.272000000000006</v>
       </c>
@@ -560,16 +558,14 @@
       <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <f>F4/G4</f>
         <v>0.98785942492012457</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <f>H4/I4</f>
         <v>0.99618016870920734</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
       <c r="F4">
         <v>3.0919999999999899</v>
       </c>
@@ -587,19 +583,18 @@
       <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <f>F5/G5</f>
         <v>0.94560729544393962</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <f>H5/I5</f>
         <v>0.94147497466901831</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <f>J5/K5</f>
         <v>0.93816951623836053</v>
       </c>
-      <c r="E5" s="1"/>
       <c r="F5">
         <v>52.676000000000002</v>
       </c>
@@ -623,19 +618,18 @@
       <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <f>F6/G6</f>
         <v>0.97480692809477387</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <f>H6/I6</f>
         <v>0.96642316979004816</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <f>J6/K6</f>
         <v>0.9630219513884003</v>
       </c>
-      <c r="E6" s="1"/>
       <c r="F6">
         <v>78.006</v>
       </c>
@@ -659,19 +653,18 @@
       <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <f>F7/G7</f>
         <v>1.022108843537415</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <f>H7/I7</f>
         <v>0.83959532341549936</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <f>J7/K7</f>
         <v>0.99970930961032456</v>
       </c>
-      <c r="E7" s="1"/>
       <c r="F7">
         <v>2.4039999999999999</v>
       </c>
@@ -695,19 +688,18 @@
       <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
         <f>F8/G8</f>
         <v>1.013357619914997</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <f>H8/I8</f>
         <v>1.0055602998386943</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
         <f>J8/K8</f>
         <v>1.0030275708252265</v>
       </c>
-      <c r="E8" s="1"/>
       <c r="F8">
         <v>26.704000000000001</v>
       </c>
@@ -731,16 +723,14 @@
       <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9">
         <f>F9/G9</f>
         <v>0.81043956043955911</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
         <f>H9/I9</f>
         <v>0.79818502588702422</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
       <c r="F9">
         <v>11.2099999999999</v>
       </c>
@@ -758,19 +748,18 @@
       <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
         <f>F10/G10</f>
         <v>1.0087719298245628</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
         <f>H10/I10</f>
         <v>1.0014513788098693</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10">
         <f>J10/K10</f>
         <v>0.99909909909909911</v>
       </c>
-      <c r="E10" s="1"/>
       <c r="F10">
         <v>0.69</v>
       </c>
@@ -794,19 +783,18 @@
       <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11">
         <f>F11/G11</f>
         <v>0.96627841915039059</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11">
         <f>H11/I11</f>
         <v>0.94306792451666066</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11">
         <f>J11/K11</f>
         <v>0.97697435932892929</v>
       </c>
-      <c r="E11" s="1"/>
       <c r="F11">
         <f>GEOMEAN(F1:F10)</f>
         <v>14.76245737299482</v>
@@ -830,6 +818,392 @@
       <c r="K11">
         <f>GEOMEAN(K1:K10)</f>
         <v>454.65124148657458</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E6ADBD-6E2A-4A20-B756-D86DA5EED3F1}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <f>F2/G2</f>
+        <v>0.98629825717466879</v>
+      </c>
+      <c r="C2">
+        <f>H2/I2</f>
+        <v>1.0195052314302777</v>
+      </c>
+      <c r="D2">
+        <f>J2/K2</f>
+        <v>1.0169660227313349</v>
+      </c>
+      <c r="F2">
+        <v>260.43599999999998</v>
+      </c>
+      <c r="G2">
+        <v>264.05399999999997</v>
+      </c>
+      <c r="H2">
+        <v>1154.0840000000001</v>
+      </c>
+      <c r="I2">
+        <v>1132.0039999999999</v>
+      </c>
+      <c r="J2">
+        <v>4722.4179999999997</v>
+      </c>
+      <c r="K2">
+        <v>4643.634</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <f>F3/G3</f>
+        <v>1.0114035441811648</v>
+      </c>
+      <c r="C3">
+        <f>H3/I3</f>
+        <v>1.0137680439441896</v>
+      </c>
+      <c r="D3">
+        <f>J3/K3</f>
+        <v>1.0137250495130805</v>
+      </c>
+      <c r="F3">
+        <v>200.44399999999999</v>
+      </c>
+      <c r="G3">
+        <v>198.184</v>
+      </c>
+      <c r="H3">
+        <v>857.07600000000002</v>
+      </c>
+      <c r="I3">
+        <v>845.43600000000004</v>
+      </c>
+      <c r="J3">
+        <v>3554.2659999999901</v>
+      </c>
+      <c r="K3">
+        <v>3506.1439999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <f>F4/G4</f>
+        <v>1.0068058076225057</v>
+      </c>
+      <c r="C4">
+        <f>H4/I4</f>
+        <v>0.99456167065477763</v>
+      </c>
+      <c r="F4">
+        <v>8.8759999999999994</v>
+      </c>
+      <c r="G4">
+        <v>8.8159999999999901</v>
+      </c>
+      <c r="H4">
+        <v>36.576000000000001</v>
+      </c>
+      <c r="I4">
+        <v>36.775999999999897</v>
+      </c>
+      <c r="J4">
+        <v>296.02999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <f>F5/G5</f>
+        <v>1.1340405873250883</v>
+      </c>
+      <c r="C5">
+        <f>H5/I5</f>
+        <v>1.1219598370227091</v>
+      </c>
+      <c r="D5">
+        <f>J5/K5</f>
+        <v>1.104469074268392</v>
+      </c>
+      <c r="F5">
+        <v>203.744</v>
+      </c>
+      <c r="G5">
+        <v>179.66200000000001</v>
+      </c>
+      <c r="H5">
+        <v>895.49</v>
+      </c>
+      <c r="I5">
+        <v>798.147999999999</v>
+      </c>
+      <c r="J5">
+        <v>3637.6439999999998</v>
+      </c>
+      <c r="K5">
+        <v>3293.5680000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <f>F6/G6</f>
+        <v>1.0020680518305491</v>
+      </c>
+      <c r="C6">
+        <f>H6/I6</f>
+        <v>1.0029247972391784</v>
+      </c>
+      <c r="D6">
+        <f>J6/K6</f>
+        <v>0.99331684025565581</v>
+      </c>
+      <c r="F6">
+        <v>372.13200000000001</v>
+      </c>
+      <c r="G6">
+        <v>371.36399999999998</v>
+      </c>
+      <c r="H6">
+        <v>1543.7539999999999</v>
+      </c>
+      <c r="I6">
+        <v>1539.252</v>
+      </c>
+      <c r="J6">
+        <v>6080.4459999999999</v>
+      </c>
+      <c r="K6">
+        <v>6121.3559999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <f>F7/G7</f>
+        <v>1.0615065653075328</v>
+      </c>
+      <c r="C7">
+        <f>H7/I7</f>
+        <v>1.0188256118323844</v>
+      </c>
+      <c r="D7">
+        <f>J7/K7</f>
+        <v>1.004227032935167</v>
+      </c>
+      <c r="F7">
+        <v>6.1440000000000001</v>
+      </c>
+      <c r="G7">
+        <v>5.7880000000000003</v>
+      </c>
+      <c r="H7">
+        <v>271.678</v>
+      </c>
+      <c r="I7">
+        <v>266.65800000000002</v>
+      </c>
+      <c r="J7">
+        <v>720.31999999999903</v>
+      </c>
+      <c r="K7">
+        <v>717.28799999999899</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <f>F8/G8</f>
+        <v>0.99746788990825697</v>
+      </c>
+      <c r="C8">
+        <f>H8/I8</f>
+        <v>0.99505433781543096</v>
+      </c>
+      <c r="D8">
+        <f>J8/K8</f>
+        <v>0.99654166166461966</v>
+      </c>
+      <c r="F8">
+        <v>54.362000000000002</v>
+      </c>
+      <c r="G8">
+        <v>54.5</v>
+      </c>
+      <c r="H8">
+        <v>216.08599999999899</v>
+      </c>
+      <c r="I8">
+        <v>217.16</v>
+      </c>
+      <c r="J8">
+        <v>863.31600000000003</v>
+      </c>
+      <c r="K8">
+        <v>866.31200000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <f>F9/G9</f>
+        <v>0.98387551049147648</v>
+      </c>
+      <c r="C9">
+        <f>H9/I9</f>
+        <v>1.0326474170014681</v>
+      </c>
+      <c r="F9">
+        <v>27.945999999999898</v>
+      </c>
+      <c r="G9">
+        <v>28.404</v>
+      </c>
+      <c r="H9">
+        <v>362.92599999999999</v>
+      </c>
+      <c r="I9">
+        <v>351.452</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <f>F10/G10</f>
+        <v>1.0011627906976743</v>
+      </c>
+      <c r="C10">
+        <f>H10/I10</f>
+        <v>0.88006439495572963</v>
+      </c>
+      <c r="D10">
+        <f>J10/K10</f>
+        <v>0.94804762855052227</v>
+      </c>
+      <c r="F10">
+        <v>1.722</v>
+      </c>
+      <c r="G10">
+        <v>1.72</v>
+      </c>
+      <c r="H10">
+        <v>6.56</v>
+      </c>
+      <c r="I10">
+        <v>7.45399999999999</v>
+      </c>
+      <c r="J10">
+        <v>28.504000000000001</v>
+      </c>
+      <c r="K10">
+        <v>30.065999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <f>F11/G11</f>
+        <v>1.0195484249989786</v>
+      </c>
+      <c r="C11">
+        <f>H11/I11</f>
+        <v>1.0070910477890023</v>
+      </c>
+      <c r="D11">
+        <f>J11/K11</f>
+        <v>0.83884178253288399</v>
+      </c>
+      <c r="F11">
+        <f>GEOMEAN(F1:F10)</f>
+        <v>43.560020186939845</v>
+      </c>
+      <c r="G11">
+        <f>GEOMEAN(G1:G10)</f>
+        <v>42.72481730034891</v>
+      </c>
+      <c r="H11">
+        <f>GEOMEAN(H1:H10)</f>
+        <v>267.40288675198167</v>
+      </c>
+      <c r="I11">
+        <f>GEOMEAN(I1:I10)</f>
+        <v>265.52007123789446</v>
+      </c>
+      <c r="J11">
+        <f>GEOMEAN(J1:J10)</f>
+        <v>1086.9281775914478</v>
+      </c>
+      <c r="K11">
+        <f>GEOMEAN(K1:K10)</f>
+        <v>1295.7487338189885</v>
       </c>
     </row>
   </sheetData>

</xml_diff>